<commit_message>
Se añadio soporte completo para menciones
</commit_message>
<xml_diff>
--- a/web/resources/uploads/planilla_seguimiento_anual.xlsx
+++ b/web/resources/uploads/planilla_seguimiento_anual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tincho\Projects\orion\web\resources\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D201AEE8-3B78-4A3C-994F-447F385AD136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAC6FD4-2237-4D16-91B6-068BF10669D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>APELLIDOS Y NOMBRES</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Vo. Bo. DIR. ACADEMICA</t>
   </si>
   <si>
-    <t>3er Parcial</t>
-  </si>
-  <si>
     <t>NOMBRE DEL DOCENTE</t>
   </si>
   <si>
@@ -194,6 +191,12 @@
   <si>
     <t>Puntaje
 4to PARCIAL</t>
+  </si>
+  <si>
+    <t>4to. Parcial</t>
+  </si>
+  <si>
+    <t>3er. Parcial</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -597,6 +600,234 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -654,230 +885,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1227,10 +1234,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Hoja12"/>
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,53 +1257,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="41"/>
+    </row>
+    <row r="2" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
+    </row>
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="79"/>
-    </row>
-    <row r="2" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="82"/>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="85"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="47"/>
     </row>
     <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
@@ -1314,73 +1321,73 @@
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="86" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="95" t="s">
+      <c r="A5" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="96"/>
-      <c r="F5" s="97" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="98"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
       <c r="K5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="99" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" s="100"/>
+      <c r="L5" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="62"/>
     </row>
     <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="101" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="102"/>
-      <c r="F6" s="71" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="72"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
       <c r="K6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="71" t="s">
+      <c r="L6" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="66"/>
+    </row>
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="M6" s="72"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="92"/>
-      <c r="B7" s="93"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="101" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="102"/>
-      <c r="F7" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="M7" s="13"/>
     </row>
@@ -1400,68 +1407,68 @@
       <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="69" t="s">
+      <c r="G9" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="46"/>
-      <c r="K9" s="67" t="s">
+      <c r="J9" s="103"/>
+      <c r="K9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="69" t="s">
+      <c r="L9" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="69" t="s">
+      <c r="M9" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="104"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="70"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="93"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>-1</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D11" s="1">
         <v>-12</v>
@@ -1478,16 +1485,16 @@
       <c r="H11" s="26">
         <v>-50</v>
       </c>
-      <c r="I11" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="45"/>
+      <c r="I11" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="102"/>
       <c r="K11" s="17">
         <v>-51</v>
       </c>
       <c r="L11" s="17"/>
       <c r="M11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1510,99 +1517,99 @@
         <v>18</v>
       </c>
       <c r="B13" s="74"/>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="51"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="81"/>
       <c r="F13" s="34">
         <v>-100</v>
       </c>
-      <c r="G13" s="105"/>
-      <c r="H13" s="64" t="s">
+      <c r="G13" s="36"/>
+      <c r="H13" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="66"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="77"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="52" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
       <c r="F14" s="34">
         <v>-101</v>
       </c>
-      <c r="G14" s="105"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="57"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="85"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="51"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="81"/>
       <c r="F15" s="34">
         <v>-102</v>
       </c>
-      <c r="G15" s="105"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="88"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
       <c r="B16" s="30"/>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
       <c r="F16" s="34">
         <v>-103</v>
       </c>
-      <c r="G16" s="105"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="60"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="88"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="81"/>
       <c r="F17" s="34">
         <v>-104</v>
       </c>
-      <c r="G17" s="105"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="63"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="91"/>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
     </row>
@@ -1627,18 +1634,18 @@
       <c r="C19" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="48"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="41" t="s">
+      <c r="E19" s="105"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
     </row>
@@ -1648,14 +1655,14 @@
       <c r="C20" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="98"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="98"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
     </row>
@@ -1665,14 +1672,14 @@
       <c r="C21" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
     </row>
@@ -1680,37 +1687,35 @@
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
+        <v>47</v>
+      </c>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="99"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="C23" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="99"/>
+      <c r="K23" s="99"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
@@ -1726,49 +1731,99 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+    </row>
+    <row r="26" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="37" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" s="37"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="28" spans="1:18" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.3"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="29" spans="1:18" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="47">
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="H14:K17"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I9:J10"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A1:M2"/>
     <mergeCell ref="A3:M3"/>
@@ -1785,35 +1840,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="L9:L10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="H14:K17"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78740157480314965" right="0.59055118110236227" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>

</xml_diff>

<commit_message>
Se añadio el Reporte Seguimiento Academico
</commit_message>
<xml_diff>
--- a/web/resources/uploads/planilla_seguimiento_anual.xlsx
+++ b/web/resources/uploads/planilla_seguimiento_anual.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tincho\Projects\orion\web\resources\uploads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAC6FD4-2237-4D16-91B6-068BF10669D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="696"/>
   </bookViews>
   <sheets>
     <sheet name="Pla. Seg." sheetId="27" r:id="rId1"/>
@@ -33,14 +27,14 @@
     <definedName name="MEICOD_200">#REF!</definedName>
     <definedName name="PRIMERO">#REF!</definedName>
     <definedName name="PRIMERO_1">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Pla. Seg.'!$1:$10</definedName>
     <definedName name="QUINTO">#REF!</definedName>
     <definedName name="SEGUNDO">#REF!</definedName>
     <definedName name="SEMESTRE">#REF!</definedName>
     <definedName name="SEXTO">#REF!</definedName>
     <definedName name="TERCERO">#REF!</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Pla. Seg.'!$1:$10</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="124519"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -75,9 +69,6 @@
     <t>FECHA  DE ENTREGA</t>
   </si>
   <si>
-    <t>PROMEDIO SEMESTRAL</t>
-  </si>
-  <si>
     <t>CODIGO:</t>
   </si>
   <si>
@@ -197,13 +188,16 @@
   </si>
   <si>
     <t>3er. Parcial</t>
+  </si>
+  <si>
+    <t>PROMEDIO ANUAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +766,74 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -780,14 +842,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -825,73 +879,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -913,7 +907,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -955,7 +949,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -987,27 +981,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1039,24 +1015,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1232,33 +1190,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja12"/>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="7.44140625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="6.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="7.42578125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="6.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" customWidth="1"/>
     <col min="9" max="9" width="12" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7.88671875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="11.44140625" style="3"/>
+    <col min="10" max="10" width="7.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="9" customHeight="1">
       <c r="A1" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -1273,7 +1231,7 @@
       <c r="L1" s="40"/>
       <c r="M1" s="41"/>
     </row>
-    <row r="2" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="6.75" customHeight="1">
       <c r="A2" s="42"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -1288,9 +1246,9 @@
       <c r="L2" s="43"/>
       <c r="M2" s="44"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1">
       <c r="A3" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
@@ -1305,7 +1263,7 @@
       <c r="L3" s="46"/>
       <c r="M3" s="47"/>
     </row>
-    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="14.25" customHeight="1">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -1320,9 +1278,9 @@
       <c r="L4" s="27"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="36" customHeight="1">
       <c r="A5" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="50"/>
@@ -1331,30 +1289,30 @@
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="59"/>
       <c r="H5" s="59"/>
       <c r="I5" s="59"/>
       <c r="J5" s="60"/>
       <c r="K5" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L5" s="61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M5" s="62"/>
     </row>
-    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" s="51"/>
       <c r="B6" s="52"/>
       <c r="C6" s="53"/>
       <c r="D6" s="63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="65"/>
       <c r="H6" s="65"/>
@@ -1364,11 +1322,11 @@
         <v>3</v>
       </c>
       <c r="L6" s="65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" s="66"/>
     </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="14.25" customHeight="1">
       <c r="A7" s="54"/>
       <c r="B7" s="55"/>
       <c r="C7" s="56"/>
@@ -1377,21 +1335,21 @@
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="65" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="65"/>
       <c r="H7" s="65"/>
       <c r="I7" s="65"/>
       <c r="J7" s="65"/>
       <c r="K7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1406,69 +1364,69 @@
       <c r="L8" s="14"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="78" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="67" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="F9" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="G9" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="92" t="s">
+      <c r="J9" s="82"/>
+      <c r="K9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="103"/>
-      <c r="K9" s="69" t="s">
+      <c r="L9" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="67" t="s">
+      <c r="M9" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="67" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:13" ht="64.5" customHeight="1">
       <c r="A10" s="72"/>
-      <c r="B10" s="93"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="68"/>
       <c r="D10" s="70"/>
       <c r="E10" s="70"/>
       <c r="F10" s="70"/>
       <c r="G10" s="70"/>
       <c r="H10" s="68"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="104"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="83"/>
       <c r="K10" s="70"/>
       <c r="L10" s="68"/>
       <c r="M10" s="68"/>
     </row>
-    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="16">
         <v>-1</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D11" s="1">
         <v>-12</v>
@@ -1485,19 +1443,19 @@
       <c r="H11" s="26">
         <v>-50</v>
       </c>
-      <c r="I11" s="101" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="102"/>
+      <c r="I11" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="81"/>
       <c r="K11" s="17">
         <v>-51</v>
       </c>
       <c r="L11" s="17"/>
       <c r="M11" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="25.5" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="18"/>
@@ -1512,22 +1470,22 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="80"/>
-      <c r="E13" s="81"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="94"/>
       <c r="F13" s="34">
         <v>-100</v>
       </c>
       <c r="G13" s="36"/>
       <c r="H13" s="75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="76"/>
       <c r="J13" s="76"/>
@@ -1535,85 +1493,85 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
       <c r="F14" s="34">
         <v>-101</v>
       </c>
       <c r="G14" s="36"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="85"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="100"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="21"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="80" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="81"/>
+      <c r="C15" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="93"/>
+      <c r="E15" s="94"/>
       <c r="F15" s="34">
         <v>-102</v>
       </c>
       <c r="G15" s="36"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="88"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="103"/>
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" s="21"/>
       <c r="B16" s="30"/>
-      <c r="C16" s="81" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
+      <c r="C16" s="94" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="97"/>
+      <c r="E16" s="97"/>
       <c r="F16" s="34">
         <v>-103</v>
       </c>
       <c r="G16" s="36"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="88"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="103"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18">
       <c r="A17" s="23"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="81"/>
+      <c r="C17" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="93"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="34">
         <v>-104</v>
       </c>
       <c r="G17" s="36"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="90"/>
-      <c r="J17" s="90"/>
-      <c r="K17" s="91"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="106"/>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1628,96 +1586,96 @@
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="E19" s="91"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="105"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="98" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="98"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="95"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="97"/>
-      <c r="H21" s="97"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="95"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="99"/>
-      <c r="J22" s="99"/>
-      <c r="K22" s="99"/>
+        <v>46</v>
+      </c>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="95"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="99"/>
-      <c r="J23" s="99"/>
-      <c r="K23" s="99"/>
+        <v>45</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1736,7 +1694,7 @@
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1751,46 +1709,46 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
     </row>
-    <row r="26" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="14.25" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="32"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="100" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="100"/>
+      <c r="D26" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="100"/>
-      <c r="K26" s="100"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18">
       <c r="A27" s="9"/>
       <c r="B27" s="33" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="9"/>
-      <c r="D27" s="94" t="s">
+      <c r="D27" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="84"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="94"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="94"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="94"/>
+      <c r="K27" s="84"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="29" spans="1:18" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:18" ht="0.75" customHeight="1"/>
+    <row r="30" spans="1:18" hidden="1"/>
   </sheetData>
   <mergeCells count="47">
     <mergeCell ref="D19:H19"/>
@@ -1798,6 +1756,11 @@
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="D23:H23"/>
     <mergeCell ref="I23:K23"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="H14:K17"/>
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="J27:K27"/>
     <mergeCell ref="D20:H20"/>
@@ -1808,11 +1771,6 @@
     <mergeCell ref="I22:K22"/>
     <mergeCell ref="D26:H26"/>
     <mergeCell ref="J26:K26"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="H14:K17"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="A13:B13"/>

</xml_diff>